<commit_message>
:scroll: JavaScript Beauty :scroll:
-Got JavaScript to output Zodiac by year :diamond_shape_with_a_dot_inside:
-Removed unncessesary CSS
-Shortened Welcome Menu code
-Added event listeners
-Created all objects
-Created formula to get Zodiac by year
</commit_message>
<xml_diff>
--- a/zodiac/docs/Year Alg.xlsx
+++ b/zodiac/docs/Year Alg.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hunter/Documents/Drexel/Scripting/idm231-hmh84/zodiac/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FEF7FD2-77C2-E84E-865A-5D2333ED647D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC2F9F4-1890-434B-97F7-4400C12493DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6680" yWindow="460" windowWidth="22120" windowHeight="17540" xr2:uid="{AB0C1237-700C-5D4B-8F6B-9E1F2FB0DFCA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="10000" windowHeight="17540" xr2:uid="{AB0C1237-700C-5D4B-8F6B-9E1F2FB0DFCA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -429,7 +429,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>